<commit_message>
Likitha Seriti WorkFlow Automation.
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Likhitha\Downloads\zee5_updated\zee5_updated\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Likhitha\git\marquisfinance\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738B644D-53E0-4686-A0C5-F48479C7A5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08EBCD7-622E-413F-9960-0B9623ED7A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="90" windowWidth="17520" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t>Create Customer Form</t>
   </si>
@@ -57,27 +57,15 @@
     <t>Finance/Cash Deal</t>
   </si>
   <si>
-    <t>CASH</t>
-  </si>
-  <si>
     <t>Add New Client Details</t>
   </si>
   <si>
     <t>First Name</t>
   </si>
   <si>
-    <t>MPANGASE</t>
-  </si>
-  <si>
-    <t>MPONISO</t>
-  </si>
-  <si>
     <t>Client Title</t>
   </si>
   <si>
-    <t xml:space="preserve"> MR</t>
-  </si>
-  <si>
     <t>ID Type</t>
   </si>
   <si>
@@ -108,9 +96,6 @@
     <t>Mob contract type</t>
   </si>
   <si>
-    <t>Prepaid</t>
-  </si>
-  <si>
     <t>Phy addr line 1</t>
   </si>
   <si>
@@ -177,10 +162,112 @@
     <t>MOBILE</t>
   </si>
   <si>
-    <t>PASSPORT</t>
-  </si>
-  <si>
-    <t>BELGIUM</t>
+    <t>RSA ID</t>
+  </si>
+  <si>
+    <t>client email</t>
+  </si>
+  <si>
+    <t>tester123@gmail.com</t>
+  </si>
+  <si>
+    <t>0875555555</t>
+  </si>
+  <si>
+    <t>080</t>
+  </si>
+  <si>
+    <t>PREPAID</t>
+  </si>
+  <si>
+    <t>0600777</t>
+  </si>
+  <si>
+    <t>HERMIA</t>
+  </si>
+  <si>
+    <t>NKOSI</t>
+  </si>
+  <si>
+    <t>4305045052080</t>
+  </si>
+  <si>
+    <t>FINANCE</t>
+  </si>
+  <si>
+    <t>Vehicle Chasis</t>
+  </si>
+  <si>
+    <t>123456789123356</t>
+  </si>
+  <si>
+    <t>EngineNumber</t>
+  </si>
+  <si>
+    <t>23421</t>
+  </si>
+  <si>
+    <t>Registration Number</t>
+  </si>
+  <si>
+    <t>2332</t>
+  </si>
+  <si>
+    <t>Vehicle Code</t>
+  </si>
+  <si>
+    <t>00815170</t>
+  </si>
+  <si>
+    <t>sellingPrice</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>02 Dec 2016</t>
+  </si>
+  <si>
+    <t>firstRegDate</t>
+  </si>
+  <si>
+    <t>interestRate</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>500000</t>
+  </si>
+  <si>
+    <t>350000</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>vehicle Condition</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Odometer</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Vehicle Use</t>
+  </si>
+  <si>
+    <t>Agreement Type</t>
+  </si>
+  <si>
+    <t>Instalment Vlaue</t>
   </si>
 </sst>
 </file>
@@ -237,15 +324,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -530,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,22 +634,22 @@
     <col min="7" max="7" width="17.7265625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="12" max="12" width="17.08984375" customWidth="1"/>
-    <col min="13" max="13" width="16.08984375" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="G1" s="6" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="G1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="L1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
@@ -569,10 +660,10 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M2" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
@@ -586,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="M3" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -597,10 +688,10 @@
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -611,10 +702,10 @@
         <v>8</v>
       </c>
       <c r="L5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -622,82 +713,80 @@
         <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="4">
-        <v>9208060255080</v>
+        <v>14</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="3">
-        <v>23520</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M8" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10">
-        <v>9886327765</v>
+        <v>19</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L12" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12">
-        <v>2572080</v>
+        <v>21</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="M14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="M15">
         <v>157</v>
@@ -705,98 +794,195 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="M16" s="3">
         <v>29729</v>
       </c>
     </row>
-    <row r="17" spans="12:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:13" ht="29" x14ac:dyDescent="0.35">
       <c r="L17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L18" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" t="s">
         <v>32</v>
       </c>
-      <c r="M17" s="2" t="s">
+    </row>
+    <row r="20" spans="10:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="L20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L18" t="s">
+      <c r="M20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M18" t="s">
+    </row>
+    <row r="21" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L19" t="s">
+      <c r="M21" t="s">
         <v>36</v>
       </c>
-      <c r="M19" t="s">
+    </row>
+    <row r="22" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L22" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="12:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="L20" t="s">
+      <c r="M22" s="3">
+        <v>33381</v>
+      </c>
+    </row>
+    <row r="23" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L23" t="s">
         <v>38</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M23" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L24" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L21" t="s">
+      <c r="M24" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="J25" s="5"/>
+      <c r="L25" t="s">
         <v>40</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M25" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L26" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L22" t="s">
+      <c r="M26" t="s">
         <v>42</v>
       </c>
-      <c r="M22" s="3">
-        <v>29729</v>
-      </c>
-    </row>
-    <row r="23" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L23" t="s">
+    </row>
+    <row r="27" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L27" t="s">
         <v>43</v>
       </c>
-      <c r="M23">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L24" t="s">
+      <c r="M27" t="s">
         <v>44</v>
       </c>
-      <c r="M24">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="25" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L25" t="s">
-        <v>45</v>
-      </c>
-      <c r="M25">
-        <v>350000</v>
-      </c>
-    </row>
-    <row r="26" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L26" t="s">
+    </row>
+    <row r="28" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L28" t="s">
         <v>46</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M28" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L27" t="s">
-        <v>48</v>
-      </c>
-      <c r="M27" t="s">
-        <v>49</v>
+    <row r="29" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L29" t="s">
+        <v>56</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L30" t="s">
+        <v>58</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L31" t="s">
+        <v>60</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="10:13" x14ac:dyDescent="0.35">
+      <c r="L32" t="s">
+        <v>62</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L33" t="s">
+        <v>64</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L34" t="s">
+        <v>67</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L35" t="s">
+        <v>68</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L36" t="s">
+        <v>74</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L37" t="s">
+        <v>76</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L38" t="s">
+        <v>78</v>
+      </c>
+      <c r="M38" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L39" t="s">
+        <v>79</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -804,7 +990,10 @@
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="L1:N1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="M28" r:id="rId1" xr:uid="{BE29E135-5DF6-4EBC-975D-AD8FE4853FDA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit as per Review Comments.
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Likhitha\git\marquisfinance\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08EBCD7-622E-413F-9960-0B9623ED7A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008E5973-8B74-4092-ADD7-52BF3D866CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="90" windowWidth="17520" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
   <si>
     <t>Create Customer Form</t>
   </si>
@@ -268,6 +268,18 @@
   </si>
   <si>
     <t>Instalment Vlaue</t>
+  </si>
+  <si>
+    <t>Bank Account Number</t>
+  </si>
+  <si>
+    <t>12376546783</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>AFRICAN BANK LIMITED</t>
   </si>
 </sst>
 </file>
@@ -324,21 +336,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -621,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="H25" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,22 +656,22 @@
     <col min="7" max="7" width="17.7265625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="12" max="12" width="17.08984375" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="G1" s="8" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="L1" s="8" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
@@ -662,7 +684,7 @@
       <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -676,7 +698,7 @@
       <c r="L3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -704,7 +726,7 @@
       <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -726,13 +748,13 @@
       <c r="L7" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L8" t="s">
         <v>16</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -740,7 +762,7 @@
       <c r="L9" t="s">
         <v>18</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -772,7 +794,7 @@
       <c r="L13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -780,7 +802,7 @@
       <c r="L14" t="s">
         <v>23</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -788,7 +810,7 @@
       <c r="L15" t="s">
         <v>25</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="7">
         <v>157</v>
       </c>
     </row>
@@ -796,7 +818,7 @@
       <c r="L16" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="8">
         <v>29729</v>
       </c>
     </row>
@@ -804,7 +826,7 @@
       <c r="L17" t="s">
         <v>27</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -812,7 +834,7 @@
       <c r="L18" t="s">
         <v>29</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -820,7 +842,7 @@
       <c r="L19" t="s">
         <v>31</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -828,7 +850,7 @@
       <c r="L20" t="s">
         <v>33</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M20" s="9" t="s">
         <v>34</v>
       </c>
     </row>
@@ -836,7 +858,7 @@
       <c r="L21" t="s">
         <v>35</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -844,7 +866,7 @@
       <c r="L22" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22" s="8">
         <v>33381</v>
       </c>
     </row>
@@ -865,7 +887,7 @@
       </c>
     </row>
     <row r="25" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J25" s="5"/>
+      <c r="J25" s="4"/>
       <c r="L25" t="s">
         <v>40</v>
       </c>
@@ -877,7 +899,7 @@
       <c r="L26" t="s">
         <v>41</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -885,7 +907,7 @@
       <c r="L27" t="s">
         <v>43</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="7" t="s">
         <v>44</v>
       </c>
     </row>
@@ -893,7 +915,7 @@
       <c r="L28" t="s">
         <v>46</v>
       </c>
-      <c r="M28" s="6" t="s">
+      <c r="M28" s="10" t="s">
         <v>47</v>
       </c>
     </row>
@@ -917,7 +939,7 @@
       <c r="L31" t="s">
         <v>60</v>
       </c>
-      <c r="M31" s="7" t="s">
+      <c r="M31" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -949,7 +971,7 @@
       <c r="L35" t="s">
         <v>68</v>
       </c>
-      <c r="M35" s="7" t="s">
+      <c r="M35" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -983,6 +1005,22 @@
       </c>
       <c r="M39" s="5" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="12:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="L40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L41" t="s">
+        <v>83</v>
+      </c>
+      <c r="M41" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit for End to End workflow.
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Likhitha\git\marquisfinance\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008E5973-8B74-4092-ADD7-52BF3D866CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E90EA4C-C2FF-4FB1-B701-7EA9A7521811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="90" windowWidth="17520" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
   <si>
     <t>Create Customer Form</t>
   </si>
@@ -222,9 +222,6 @@
     <t>sellingPrice</t>
   </si>
   <si>
-    <t>20000</t>
-  </si>
-  <si>
     <t>02 Dec 2016</t>
   </si>
   <si>
@@ -280,6 +277,27 @@
   </si>
   <si>
     <t>AFRICAN BANK LIMITED</t>
+  </si>
+  <si>
+    <t>BANK STATEMENT</t>
+  </si>
+  <si>
+    <t>DocumentUpload1</t>
+  </si>
+  <si>
+    <t>DocumentUpload2</t>
+  </si>
+  <si>
+    <t>ID DOCUMENT - CLIENT</t>
+  </si>
+  <si>
+    <t>360,000.00</t>
+  </si>
+  <si>
+    <t>Residual Amount</t>
+  </si>
+  <si>
+    <t>50,000</t>
   </si>
 </sst>
 </file>
@@ -347,9 +365,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -361,6 +376,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -643,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H25" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,22 +674,22 @@
     <col min="7" max="7" width="17.7265625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="12" max="12" width="17.08984375" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" style="7" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
     </row>
     <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
@@ -684,7 +702,7 @@
       <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>52</v>
       </c>
     </row>
@@ -698,7 +716,7 @@
       <c r="L3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>53</v>
       </c>
     </row>
@@ -713,7 +731,7 @@
         <v>12</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -726,7 +744,7 @@
       <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -748,13 +766,13 @@
       <c r="L7" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="8"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L8" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -762,7 +780,7 @@
       <c r="L9" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="7" t="s">
+      <c r="M9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -794,7 +812,7 @@
       <c r="L13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="7" t="s">
+      <c r="M13" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -802,7 +820,7 @@
       <c r="L14" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="M14" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -810,7 +828,7 @@
       <c r="L15" t="s">
         <v>25</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="6">
         <v>157</v>
       </c>
     </row>
@@ -818,7 +836,7 @@
       <c r="L16" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="8">
+      <c r="M16" s="7">
         <v>29729</v>
       </c>
     </row>
@@ -826,7 +844,7 @@
       <c r="L17" t="s">
         <v>27</v>
       </c>
-      <c r="M17" s="9" t="s">
+      <c r="M17" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -834,7 +852,7 @@
       <c r="L18" t="s">
         <v>29</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="M18" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -842,7 +860,7 @@
       <c r="L19" t="s">
         <v>31</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="M19" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -850,7 +868,7 @@
       <c r="L20" t="s">
         <v>33</v>
       </c>
-      <c r="M20" s="9" t="s">
+      <c r="M20" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -858,7 +876,7 @@
       <c r="L21" t="s">
         <v>35</v>
       </c>
-      <c r="M21" s="7" t="s">
+      <c r="M21" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -866,7 +884,7 @@
       <c r="L22" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="8">
+      <c r="M22" s="7">
         <v>33381</v>
       </c>
     </row>
@@ -875,7 +893,7 @@
         <v>38</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="10:13" x14ac:dyDescent="0.35">
@@ -883,7 +901,7 @@
         <v>39</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="10:13" x14ac:dyDescent="0.35">
@@ -892,14 +910,14 @@
         <v>40</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L26" t="s">
         <v>41</v>
       </c>
-      <c r="M26" s="7" t="s">
+      <c r="M26" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -907,7 +925,7 @@
       <c r="L27" t="s">
         <v>43</v>
       </c>
-      <c r="M27" s="7" t="s">
+      <c r="M27" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -915,7 +933,7 @@
       <c r="L28" t="s">
         <v>46</v>
       </c>
-      <c r="M28" s="10" t="s">
+      <c r="M28" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -956,44 +974,44 @@
         <v>64</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L35" t="s">
+        <v>67</v>
+      </c>
+      <c r="M35" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="36" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L36" t="s">
+        <v>73</v>
+      </c>
+      <c r="M36" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="37" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L37" t="s">
+        <v>75</v>
+      </c>
+      <c r="M37" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="38" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>6</v>
@@ -1001,26 +1019,50 @@
     </row>
     <row r="39" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L39" t="s">
+        <v>78</v>
+      </c>
+      <c r="M39" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="40" spans="12:13" ht="29" x14ac:dyDescent="0.35">
       <c r="L40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M40" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="41" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L41" t="s">
+        <v>82</v>
+      </c>
+      <c r="M41" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M41" s="7" t="s">
+    </row>
+    <row r="42" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L42" t="s">
+        <v>85</v>
+      </c>
+      <c r="M42" s="5" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L43" t="s">
+        <v>86</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L44" t="s">
+        <v>89</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'LikhithaIGS' into 'master'"
This reverts merge request !10
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Likhitha\git\marquisfinance\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E90EA4C-C2FF-4FB1-B701-7EA9A7521811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08EBCD7-622E-413F-9960-0B9623ED7A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="90" windowWidth="17520" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t>Create Customer Form</t>
   </si>
@@ -222,6 +222,9 @@
     <t>sellingPrice</t>
   </si>
   <si>
+    <t>20000</t>
+  </si>
+  <si>
     <t>02 Dec 2016</t>
   </si>
   <si>
@@ -265,39 +268,6 @@
   </si>
   <si>
     <t>Instalment Vlaue</t>
-  </si>
-  <si>
-    <t>Bank Account Number</t>
-  </si>
-  <si>
-    <t>12376546783</t>
-  </si>
-  <si>
-    <t>Bank Name</t>
-  </si>
-  <si>
-    <t>AFRICAN BANK LIMITED</t>
-  </si>
-  <si>
-    <t>BANK STATEMENT</t>
-  </si>
-  <si>
-    <t>DocumentUpload1</t>
-  </si>
-  <si>
-    <t>DocumentUpload2</t>
-  </si>
-  <si>
-    <t>ID DOCUMENT - CLIENT</t>
-  </si>
-  <si>
-    <t>360,000.00</t>
-  </si>
-  <si>
-    <t>Residual Amount</t>
-  </si>
-  <si>
-    <t>50,000</t>
   </si>
 </sst>
 </file>
@@ -354,27 +324,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -661,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N44"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,22 +634,22 @@
     <col min="7" max="7" width="17.7265625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="12" max="12" width="17.08984375" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="G1" s="10" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="G1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="L1" s="10" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
@@ -702,7 +662,7 @@
       <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -716,7 +676,7 @@
       <c r="L3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -731,7 +691,7 @@
         <v>12</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -744,7 +704,7 @@
       <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -766,13 +726,13 @@
       <c r="L7" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="7"/>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L8" t="s">
         <v>16</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -780,7 +740,7 @@
       <c r="L9" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -812,7 +772,7 @@
       <c r="L13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="M13" t="s">
         <v>50</v>
       </c>
     </row>
@@ -820,7 +780,7 @@
       <c r="L14" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="M14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -828,7 +788,7 @@
       <c r="L15" t="s">
         <v>25</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M15">
         <v>157</v>
       </c>
     </row>
@@ -836,7 +796,7 @@
       <c r="L16" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="3">
         <v>29729</v>
       </c>
     </row>
@@ -844,7 +804,7 @@
       <c r="L17" t="s">
         <v>27</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -852,7 +812,7 @@
       <c r="L18" t="s">
         <v>29</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="M18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -860,7 +820,7 @@
       <c r="L19" t="s">
         <v>31</v>
       </c>
-      <c r="M19" s="6" t="s">
+      <c r="M19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -868,7 +828,7 @@
       <c r="L20" t="s">
         <v>33</v>
       </c>
-      <c r="M20" s="8" t="s">
+      <c r="M20" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -876,7 +836,7 @@
       <c r="L21" t="s">
         <v>35</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="M21" t="s">
         <v>36</v>
       </c>
     </row>
@@ -884,7 +844,7 @@
       <c r="L22" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="3">
         <v>33381</v>
       </c>
     </row>
@@ -893,7 +853,7 @@
         <v>38</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="10:13" x14ac:dyDescent="0.35">
@@ -901,23 +861,23 @@
         <v>39</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J25" s="4"/>
+      <c r="J25" s="5"/>
       <c r="L25" t="s">
         <v>40</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L26" t="s">
         <v>41</v>
       </c>
-      <c r="M26" s="6" t="s">
+      <c r="M26" t="s">
         <v>42</v>
       </c>
     </row>
@@ -925,7 +885,7 @@
       <c r="L27" t="s">
         <v>43</v>
       </c>
-      <c r="M27" s="6" t="s">
+      <c r="M27" t="s">
         <v>44</v>
       </c>
     </row>
@@ -933,7 +893,7 @@
       <c r="L28" t="s">
         <v>46</v>
       </c>
-      <c r="M28" s="9" t="s">
+      <c r="M28" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -957,7 +917,7 @@
       <c r="L31" t="s">
         <v>60</v>
       </c>
-      <c r="M31" s="5" t="s">
+      <c r="M31" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -974,44 +934,44 @@
         <v>64</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L34" t="s">
+        <v>67</v>
+      </c>
+      <c r="M34" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="35" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L35" t="s">
-        <v>67</v>
-      </c>
-      <c r="M35" s="5" t="s">
         <v>68</v>
+      </c>
+      <c r="M35" s="7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L37" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>6</v>
@@ -1019,50 +979,10 @@
     </row>
     <row r="39" spans="12:13" x14ac:dyDescent="0.35">
       <c r="L39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="12:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="L40" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L41" t="s">
-        <v>82</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L42" t="s">
-        <v>85</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L43" t="s">
-        <v>86</v>
-      </c>
-      <c r="M43" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L44" t="s">
-        <v>89</v>
-      </c>
-      <c r="M44" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Took project from folder and reworked again.
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Likhitha\git\marquisfinance\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08EBCD7-622E-413F-9960-0B9623ED7A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EC26D2-F05B-4955-BB0C-0D6439BFFEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="90" windowWidth="17520" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
   <si>
     <t>Create Customer Form</t>
   </si>
@@ -267,7 +267,31 @@
     <t>Agreement Type</t>
   </si>
   <si>
-    <t>Instalment Vlaue</t>
+    <t>Bank Account Number</t>
+  </si>
+  <si>
+    <t>12376546783</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>AFRICAN BANK LIMITED</t>
+  </si>
+  <si>
+    <t>BANK STATEMENT</t>
+  </si>
+  <si>
+    <t>DocumentUpload1</t>
+  </si>
+  <si>
+    <t>DocumentUpload2</t>
+  </si>
+  <si>
+    <t>ID DOCUMENT - CLIENT</t>
+  </si>
+  <si>
+    <t>INSTALMENT SALE</t>
   </si>
 </sst>
 </file>
@@ -324,17 +348,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -621,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F33" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,22 +668,22 @@
     <col min="7" max="7" width="17.7265625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="12" max="12" width="17.08984375" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="G1" s="8" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="G1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="L1" s="8" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
     </row>
     <row r="2" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
@@ -662,7 +696,7 @@
       <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="6" t="s">
         <v>52</v>
       </c>
     </row>
@@ -676,7 +710,7 @@
       <c r="L3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="6" t="s">
         <v>53</v>
       </c>
     </row>
@@ -704,7 +738,7 @@
       <c r="L5" t="s">
         <v>13</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -726,13 +760,13 @@
       <c r="L7" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L8" t="s">
         <v>16</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -740,7 +774,7 @@
       <c r="L9" t="s">
         <v>18</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -772,7 +806,7 @@
       <c r="L13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -780,7 +814,7 @@
       <c r="L14" t="s">
         <v>23</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -788,7 +822,7 @@
       <c r="L15" t="s">
         <v>25</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="6">
         <v>157</v>
       </c>
     </row>
@@ -796,7 +830,7 @@
       <c r="L16" t="s">
         <v>26</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="7">
         <v>29729</v>
       </c>
     </row>
@@ -804,7 +838,7 @@
       <c r="L17" t="s">
         <v>27</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -812,7 +846,7 @@
       <c r="L18" t="s">
         <v>29</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -820,7 +854,7 @@
       <c r="L19" t="s">
         <v>31</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -828,7 +862,7 @@
       <c r="L20" t="s">
         <v>33</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M20" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -836,7 +870,7 @@
       <c r="L21" t="s">
         <v>35</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -844,7 +878,7 @@
       <c r="L22" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22" s="7">
         <v>33381</v>
       </c>
     </row>
@@ -865,7 +899,7 @@
       </c>
     </row>
     <row r="25" spans="10:13" x14ac:dyDescent="0.35">
-      <c r="J25" s="5"/>
+      <c r="J25" s="4"/>
       <c r="L25" t="s">
         <v>40</v>
       </c>
@@ -877,7 +911,7 @@
       <c r="L26" t="s">
         <v>41</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -885,7 +919,7 @@
       <c r="L27" t="s">
         <v>43</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -893,7 +927,7 @@
       <c r="L28" t="s">
         <v>46</v>
       </c>
-      <c r="M28" s="6" t="s">
+      <c r="M28" s="9" t="s">
         <v>47</v>
       </c>
     </row>
@@ -917,7 +951,7 @@
       <c r="L31" t="s">
         <v>60</v>
       </c>
-      <c r="M31" s="7" t="s">
+      <c r="M31" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -949,7 +983,7 @@
       <c r="L35" t="s">
         <v>68</v>
       </c>
-      <c r="M35" s="7" t="s">
+      <c r="M35" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -982,7 +1016,39 @@
         <v>79</v>
       </c>
       <c r="M39" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="12:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="L40" s="2" t="s">
         <v>80</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L41" t="s">
+        <v>82</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L42" t="s">
+        <v>85</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="12:13" x14ac:dyDescent="0.35">
+      <c r="L43" t="s">
+        <v>86</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Test Scripts for Value added Products.
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Likhitha\git\marquisfinance\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EC26D2-F05B-4955-BB0C-0D6439BFFEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B978ABD6-F473-4647-A1F2-411BEC0FE251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="90" windowWidth="17520" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="90" windowWidth="17520" windowHeight="9990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RefNumber" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="94">
   <si>
     <t>Create Customer Form</t>
   </si>
@@ -51,9 +52,6 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>Hussain</t>
-  </si>
-  <si>
     <t>Finance/Cash Deal</t>
   </si>
   <si>
@@ -198,33 +196,18 @@
     <t>Vehicle Chasis</t>
   </si>
   <si>
-    <t>123456789123356</t>
-  </si>
-  <si>
     <t>EngineNumber</t>
   </si>
   <si>
-    <t>23421</t>
-  </si>
-  <si>
     <t>Registration Number</t>
   </si>
   <si>
-    <t>2332</t>
-  </si>
-  <si>
     <t>Vehicle Code</t>
   </si>
   <si>
-    <t>00815170</t>
-  </si>
-  <si>
     <t>sellingPrice</t>
   </si>
   <si>
-    <t>20000</t>
-  </si>
-  <si>
     <t>02 Dec 2016</t>
   </si>
   <si>
@@ -234,9 +217,6 @@
     <t>interestRate</t>
   </si>
   <si>
-    <t>12.5</t>
-  </si>
-  <si>
     <t>25</t>
   </si>
   <si>
@@ -252,9 +232,6 @@
     <t>vehicle Condition</t>
   </si>
   <si>
-    <t>NEW</t>
-  </si>
-  <si>
     <t>Odometer</t>
   </si>
   <si>
@@ -292,6 +269,45 @@
   </si>
   <si>
     <t>INSTALMENT SALE</t>
+  </si>
+  <si>
+    <t>Marquis Reference Number</t>
+  </si>
+  <si>
+    <t>TMP448GP</t>
+  </si>
+  <si>
+    <t>EHSM225</t>
+  </si>
+  <si>
+    <t>AHTZZ69G805037240</t>
+  </si>
+  <si>
+    <t>26526530</t>
+  </si>
+  <si>
+    <t>360,000.00</t>
+  </si>
+  <si>
+    <t>12.75</t>
+  </si>
+  <si>
+    <t>USED</t>
+  </si>
+  <si>
+    <t>Delivery Fee</t>
+  </si>
+  <si>
+    <t>2,400</t>
+  </si>
+  <si>
+    <t>License Charge</t>
+  </si>
+  <si>
+    <t>650</t>
+  </si>
+  <si>
+    <t>2000007367</t>
   </si>
 </sst>
 </file>
@@ -655,20 +671,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="12" max="12" width="17.08984375" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.36328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.7265625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.08984375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.1796875" style="6" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -680,7 +696,7 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="L1" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
@@ -694,10 +710,10 @@
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
@@ -711,7 +727,7 @@
         <v>7</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -722,10 +738,10 @@
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -733,94 +749,94 @@
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="L5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="G6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M15" s="6">
         <v>157</v>
@@ -828,7 +844,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M16" s="7">
         <v>29729</v>
@@ -836,47 +852,47 @@
     </row>
     <row r="17" spans="10:13" ht="29" x14ac:dyDescent="0.35">
       <c r="L17" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="M17" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L18" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L19" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="10:13" ht="29" x14ac:dyDescent="0.35">
       <c r="L20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M20" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L21" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="22" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M22" s="7">
         <v>33381</v>
@@ -884,171 +900,193 @@
     </row>
     <row r="23" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="10:13" x14ac:dyDescent="0.35">
       <c r="J25" s="4"/>
       <c r="L25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L26" t="s">
+        <v>40</v>
+      </c>
+      <c r="M26" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L27" t="s">
+        <v>42</v>
+      </c>
+      <c r="M27" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="28" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M28" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="M28" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="29" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="10:13" x14ac:dyDescent="0.35">
       <c r="L32" t="s">
+        <v>58</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="L33" t="s">
+        <v>59</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="L34" t="s">
+        <v>61</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="L35" t="s">
         <v>62</v>
       </c>
-      <c r="M32" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L33" t="s">
-        <v>64</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L34" t="s">
+      <c r="M35" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="L36" t="s">
         <v>67</v>
       </c>
-      <c r="M34" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L35" t="s">
+      <c r="M36" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="L37" t="s">
         <v>68</v>
       </c>
-      <c r="M35" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L36" t="s">
-        <v>74</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L37" t="s">
-        <v>76</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="11:13" x14ac:dyDescent="0.35">
       <c r="L38" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="M38" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="12:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="11:13" x14ac:dyDescent="0.35">
       <c r="L39" t="s">
+        <v>71</v>
+      </c>
+      <c r="M39" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="11:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="L40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M40" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="L41" t="s">
+        <v>74</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="L42" t="s">
+        <v>77</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="L43" t="s">
+        <v>78</v>
+      </c>
+      <c r="M43" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M39" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="12:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="L40" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L41" t="s">
-        <v>82</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L42" t="s">
-        <v>85</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="12:13" x14ac:dyDescent="0.35">
-      <c r="L43" t="s">
-        <v>86</v>
-      </c>
-      <c r="M43" s="5" t="s">
-        <v>87</v>
+    </row>
+    <row r="44" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="K44">
+        <v>43</v>
+      </c>
+      <c r="L44" t="s">
+        <v>89</v>
+      </c>
+      <c r="M44" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="K45">
+        <v>44</v>
+      </c>
+      <c r="L45" t="s">
+        <v>91</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1062,4 +1100,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB8217E-4CD9-4CE8-B210-279243651323}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.36328125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Payout Script changes due to new code change
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backup\Jan-15th\marquisfinance\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradeep\Marquis\Master download\1-2-2023\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D7E0F3-53F6-41B8-8269-2B794A1C815A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761E9EE0-3EE1-4456-9DC3-915BB7DC7B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="90" windowWidth="17520" windowHeight="9990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="7" r:id="rId1"/>
@@ -787,19 +787,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>94</v>
       </c>
       <c r="B1" s="17"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -807,7 +807,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -834,12 +834,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="16.81640625" style="3" collapsed="1"/>
+    <col min="1" max="16384" width="16.77734375" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>102</v>
       </c>
@@ -847,7 +847,7 @@
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -990,7 +990,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>98</v>
       </c>
@@ -1131,13 +1131,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>83</v>
       </c>
       <c r="C4" s="18"/>
     </row>
-    <row r="5" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1174,83 +1174,83 @@
       <c r="S6" s="2"/>
       <c r="AN6" s="2"/>
     </row>
-    <row r="7" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G7" s="2"/>
       <c r="N7" s="6"/>
       <c r="S7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AN7" s="2"/>
     </row>
-    <row r="8" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G8" s="2"/>
       <c r="S8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AN8" s="2"/>
     </row>
-    <row r="9" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G9" s="2"/>
       <c r="S9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AN9" s="2"/>
     </row>
-    <row r="10" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G10" s="2"/>
       <c r="N10" s="4"/>
       <c r="S10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AN10" s="2"/>
     </row>
-    <row r="11" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="2"/>
       <c r="N11" s="4"/>
       <c r="S11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AN11" s="2"/>
     </row>
-    <row r="12" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G12" s="2"/>
       <c r="N12" s="4"/>
       <c r="S12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AN12" s="2"/>
     </row>
-    <row r="13" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G13" s="2"/>
       <c r="S13" s="2"/>
       <c r="AC13" s="2"/>
     </row>
-    <row r="14" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G14" s="2"/>
       <c r="S14" s="2"/>
       <c r="AC14" s="2"/>
       <c r="AN14" s="2"/>
     </row>
-    <row r="15" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G15" s="2"/>
       <c r="S15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AN15" s="2"/>
     </row>
-    <row r="16" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:47" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G16" s="2"/>
       <c r="N16" s="6"/>
       <c r="S16" s="2"/>
       <c r="AC16" s="2"/>
       <c r="AN16" s="2"/>
     </row>
-    <row r="17" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G17" s="2"/>
       <c r="S17" s="2"/>
       <c r="AC17" s="2"/>
       <c r="AN17" s="2"/>
     </row>
-    <row r="18" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G18" s="2"/>
       <c r="S18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AN18" s="2"/>
     </row>
-    <row r="19" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G19" s="2"/>
       <c r="S19" s="2"/>
       <c r="AC19" s="2"/>
@@ -1258,7 +1258,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G20" s="2"/>
       <c r="S20" s="2"/>
       <c r="AC20" s="2"/>
@@ -1266,148 +1266,148 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G21" s="2"/>
       <c r="S21" s="2"/>
       <c r="AC21" s="2"/>
     </row>
-    <row r="22" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G22" s="2"/>
       <c r="N22" s="6"/>
       <c r="S22" s="2"/>
       <c r="AC22" s="2"/>
     </row>
-    <row r="23" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G23" s="2"/>
       <c r="N23" s="4"/>
       <c r="S23" s="2"/>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G24" s="2"/>
       <c r="N24" s="4"/>
       <c r="S24" s="2"/>
       <c r="AC24" s="2"/>
     </row>
-    <row r="25" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G25" s="2"/>
       <c r="K25" s="4"/>
       <c r="N25" s="4"/>
       <c r="S25" s="2"/>
       <c r="AC25" s="2"/>
     </row>
-    <row r="26" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G26" s="2"/>
       <c r="S26" s="2"/>
     </row>
-    <row r="27" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G27" s="2"/>
       <c r="S27" s="2"/>
       <c r="AC27" s="2"/>
     </row>
-    <row r="28" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G28" s="2"/>
       <c r="N28" s="5"/>
       <c r="S28" s="2"/>
       <c r="AC28" s="2"/>
     </row>
-    <row r="29" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G29" s="2"/>
       <c r="N29" s="4"/>
       <c r="S29" s="2"/>
       <c r="AC29" s="2"/>
     </row>
-    <row r="30" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G30" s="2"/>
       <c r="N30" s="4"/>
       <c r="S30" s="2"/>
       <c r="AC30" s="2"/>
     </row>
-    <row r="31" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G31" s="2"/>
       <c r="N31" s="4"/>
       <c r="S31" s="2"/>
       <c r="AC31" s="2"/>
     </row>
-    <row r="32" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="7:40" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G32" s="2"/>
       <c r="N32" s="4"/>
       <c r="S32" s="2"/>
       <c r="AC32" s="2"/>
     </row>
-    <row r="33" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G33" s="2"/>
       <c r="N33" s="4"/>
     </row>
-    <row r="34" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G34" s="2"/>
       <c r="N34" s="4"/>
       <c r="S34" s="2"/>
     </row>
-    <row r="35" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G35" s="2"/>
       <c r="N35" s="4"/>
       <c r="S35" s="2"/>
     </row>
-    <row r="36" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G36" s="2"/>
       <c r="N36" s="4"/>
       <c r="S36" s="2"/>
     </row>
-    <row r="37" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G37" s="2"/>
       <c r="N37" s="4"/>
       <c r="S37" s="2"/>
     </row>
-    <row r="38" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G38" s="2"/>
       <c r="N38" s="4"/>
       <c r="S38" s="2"/>
     </row>
-    <row r="39" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G39" s="2"/>
       <c r="N39" s="4"/>
       <c r="S39" s="2"/>
     </row>
-    <row r="40" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G40" s="2"/>
       <c r="N40" s="4"/>
     </row>
-    <row r="41" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G42" s="2"/>
       <c r="N42" s="4"/>
     </row>
-    <row r="43" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G43" s="2"/>
       <c r="N43" s="4"/>
     </row>
-    <row r="44" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G44" s="2"/>
       <c r="N44" s="4"/>
     </row>
-    <row r="45" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N45" s="4"/>
     </row>
-    <row r="46" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G46" s="2"/>
       <c r="N46" s="4"/>
     </row>
-    <row r="47" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="7:19" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G48" s="2"/>
     </row>
-    <row r="49" spans="7:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="7:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G49" s="2"/>
     </row>
-    <row r="50" spans="7:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="7:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="7:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="7:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G51" s="2"/>
     </row>
   </sheetData>
@@ -1425,25 +1425,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB8217E-4CD9-4CE8-B210-279243651323}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.90625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2000006416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2000006844</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2000007330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commited changes on reading data from Excel using key value and multiple Run. Written  scripts for financier -police verification hack and also for Digi-Sign-partially. blocked with test data.
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XC2\marquisfinance\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA092EC8-3CFF-4550-B9C8-396C61DEFE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F77C9E-0AE9-42FF-B27D-D148BB7BEBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="90" windowWidth="17520" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="90" windowWidth="17520" windowHeight="9990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="7" r:id="rId1"/>
     <sheet name="TestDataOLD" sheetId="1" r:id="rId2"/>
     <sheet name="TestData" sheetId="9" r:id="rId3"/>
-    <sheet name="CusotmerDetails" sheetId="8" r:id="rId4"/>
+    <sheet name="old" sheetId="8" r:id="rId4"/>
     <sheet name="RefNumber" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="125">
   <si>
     <t>Dealer Group</t>
   </si>
@@ -346,34 +346,9 @@
     <t>SALARY</t>
   </si>
   <si>
-    <t>The application has succeeded. Your reference number is 2000007366.
-MQRefNo - 2000007366</t>
-  </si>
-  <si>
     <t>Test@12345</t>
   </si>
   <si>
-    <t>3434343434222</t>
-  </si>
-  <si>
-    <t>0000000000</t>
-  </si>
-  <si>
-    <t>Likhitha test1</t>
-  </si>
-  <si>
-    <t>Likhitha test2</t>
-  </si>
-  <si>
-    <t>Likhitha test3</t>
-  </si>
-  <si>
-    <t>Likhitha test4</t>
-  </si>
-  <si>
-    <t>Likhitha test5</t>
-  </si>
-  <si>
     <t>Financier Credentials</t>
   </si>
   <si>
@@ -387,6 +362,48 @@
   </si>
   <si>
     <t>userID</t>
+  </si>
+  <si>
+    <t>InterestRateType</t>
+  </si>
+  <si>
+    <t>residualAmount</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>DocumentUpload4</t>
+  </si>
+  <si>
+    <t>INSURANCE CONFIRMATION</t>
+  </si>
+  <si>
+    <t>180000</t>
+  </si>
+  <si>
+    <t>150000</t>
+  </si>
+  <si>
+    <t>27 Feb 2023</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>195,000.00</t>
+  </si>
+  <si>
+    <t>6301045178080</t>
+  </si>
+  <si>
+    <t>VENESH</t>
+  </si>
+  <si>
+    <t>SEWSUNKER</t>
+  </si>
+  <si>
+    <t>MR</t>
   </si>
 </sst>
 </file>
@@ -439,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -475,12 +492,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -558,8 +588,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -850,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F55BEF-7DB7-4FE7-917F-175DD7B48354}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -861,10 +901,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -879,28 +919,29 @@
         <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>114</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -919,13 +960,12 @@
   <dimension ref="A1:BA48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AU5" sqref="AU5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="16.81640625" style="2"/>
-    <col min="7" max="16384" width="16.81640625" style="2" collapsed="1"/>
+    <col min="1" max="16384" width="16.81640625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -1497,50 +1537,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA63286-C133-4451-909B-35F8FE7B40BE}">
-  <dimension ref="A1:AY8"/>
+  <dimension ref="A1:BB3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AZ3" sqref="AZ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" style="17" customWidth="1"/>
-    <col min="2" max="5" width="9.26953125" style="17"/>
-    <col min="6" max="6" width="21.1796875" style="17" customWidth="1"/>
-    <col min="7" max="8" width="9.26953125" style="17"/>
-    <col min="9" max="9" width="16.7265625" style="17" customWidth="1"/>
-    <col min="10" max="10" width="9.26953125" style="17"/>
-    <col min="11" max="11" width="10.1796875" style="17" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" style="17" customWidth="1"/>
-    <col min="13" max="13" width="16.36328125" style="17" customWidth="1"/>
-    <col min="14" max="14" width="13.1796875" style="17" customWidth="1"/>
-    <col min="15" max="16" width="9.26953125" style="17"/>
-    <col min="17" max="17" width="18.26953125" style="17" customWidth="1"/>
-    <col min="18" max="19" width="9.26953125" style="17"/>
-    <col min="20" max="20" width="9.26953125" style="2"/>
-    <col min="21" max="36" width="9.26953125" style="17"/>
-    <col min="37" max="37" width="11.1796875" style="17" customWidth="1"/>
-    <col min="38" max="38" width="13" style="17" customWidth="1"/>
-    <col min="39" max="39" width="17.54296875" style="17" customWidth="1"/>
-    <col min="40" max="40" width="12.08984375" style="17" customWidth="1"/>
-    <col min="41" max="41" width="16.453125" style="17" customWidth="1"/>
-    <col min="42" max="42" width="9.26953125" style="17"/>
-    <col min="43" max="43" width="16" style="17" customWidth="1"/>
-    <col min="44" max="44" width="14.54296875" style="17" customWidth="1"/>
-    <col min="45" max="46" width="9.26953125" style="17"/>
-    <col min="47" max="47" width="15.54296875" style="17" customWidth="1"/>
-    <col min="48" max="48" width="13.54296875" style="17" customWidth="1"/>
-    <col min="49" max="49" width="12.54296875" style="17" customWidth="1"/>
-    <col min="50" max="16384" width="9.26953125" style="17"/>
+    <col min="1" max="1" width="17.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="9.26953125" style="17" collapsed="1"/>
+    <col min="4" max="4" width="12.08984375" style="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.36328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.36328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="9.26953125" style="17" collapsed="1"/>
+    <col min="9" max="9" width="16.7265625" style="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.26953125" style="17" collapsed="1"/>
+    <col min="11" max="11" width="10.1796875" style="17" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.1796875" style="17" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.36328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.1796875" style="17" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="9.26953125" style="17" collapsed="1"/>
+    <col min="17" max="17" width="18.26953125" style="17" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="9.26953125" style="17" collapsed="1"/>
+    <col min="20" max="20" width="9.26953125" style="2" collapsed="1"/>
+    <col min="21" max="25" width="9.26953125" style="17" collapsed="1"/>
+    <col min="26" max="26" width="9.453125" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="32" width="9.26953125" style="17" collapsed="1"/>
+    <col min="33" max="33" width="10.6328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="9.26953125" style="17" collapsed="1"/>
+    <col min="35" max="35" width="10.7265625" style="17" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.26953125" style="17" collapsed="1"/>
+    <col min="37" max="37" width="11.1796875" style="17" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="13" style="17" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="17.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="40" max="42" width="12.08984375" style="17" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="16.453125" style="17" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="9.26953125" style="17" collapsed="1"/>
+    <col min="45" max="45" width="16" style="17" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="14.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="9.26953125" style="17" collapsed="1"/>
+    <col min="49" max="49" width="15.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="13.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="20.6328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="53" max="16384" width="9.26953125" style="17" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="F1" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:51" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
@@ -1662,40 +1711,49 @@
         <v>53</v>
       </c>
       <c r="AO2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="AQ2" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AP2" s="10" t="s">
+      <c r="AR2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AQ2" s="10" t="s">
+      <c r="AS2" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AR2" s="10" t="s">
+      <c r="AT2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AS2" s="10" t="s">
+      <c r="AU2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AT2" s="10" t="s">
+      <c r="AV2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AU2" s="10" t="s">
+      <c r="AW2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AV2" s="10" t="s">
+      <c r="AX2" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="AW2" s="10" t="s">
+      <c r="AY2" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AZ2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="AX2" s="10" t="s">
+      <c r="BA2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AY2" s="10" t="s">
+      <c r="BB2" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:51" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
@@ -1706,22 +1764,22 @@
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>97</v>
+      <c r="F3" s="27" t="s">
+        <v>122</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>40</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="10" t="s">
@@ -1770,16 +1828,16 @@
         <v>31</v>
       </c>
       <c r="Z3" s="13">
-        <v>33381</v>
+        <v>36303</v>
       </c>
       <c r="AA3" s="9" t="s">
         <v>54</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="AD3" s="10" t="s">
         <v>37</v>
@@ -1803,824 +1861,63 @@
         <v>95</v>
       </c>
       <c r="AK3" s="9" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="AL3" s="9" t="s">
         <v>94</v>
       </c>
       <c r="AM3" s="9" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="AN3" s="9" t="s">
         <v>76</v>
       </c>
       <c r="AO3" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP3" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="AP3" s="9" t="s">
+      <c r="AR3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AQ3" s="9" t="s">
+      <c r="AS3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="AR3" s="9" t="s">
+      <c r="AT3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AS3" s="10" t="s">
+      <c r="AU3" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="AT3" s="9" t="s">
+      <c r="AV3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AU3" s="9" t="s">
+      <c r="AW3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="AV3" s="10" t="s">
+      <c r="AX3" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="AW3" s="9" t="s">
+      <c r="AY3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="AZ3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="AX3" s="9" t="s">
+      <c r="BA3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AY3" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:51" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="S4" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="T4" s="13">
-        <v>41052</v>
-      </c>
-      <c r="U4" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="V4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="X4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z4" s="13">
-        <v>33381</v>
-      </c>
-      <c r="AA4" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB4" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC4" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG4" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH4" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK4" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL4" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM4" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN4" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO4" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP4" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ4" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR4" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS4" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT4" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV4" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AW4" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX4" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="AY4" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:51" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="S5" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="T5" s="13">
-        <v>41052</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="V5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y5" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z5" s="13">
-        <v>33381</v>
-      </c>
-      <c r="AA5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG5" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI5" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ5" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK5" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL5" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM5" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN5" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO5" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP5" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ5" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR5" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT5" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV5" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AW5" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX5" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="AY5" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:51" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="S6" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="T6" s="13">
-        <v>41052</v>
-      </c>
-      <c r="U6" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="V6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="W6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="X6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z6" s="13">
-        <v>33381</v>
-      </c>
-      <c r="AA6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB6" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC6" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE6" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG6" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH6" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ6" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL6" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM6" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN6" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO6" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP6" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ6" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR6" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV6" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AW6" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX6" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="AY6" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:51" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="S7" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="T7" s="13">
-        <v>41052</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="V7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="W7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="X7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z7" s="13">
-        <v>33381</v>
-      </c>
-      <c r="AA7" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB7" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG7" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH7" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI7" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ7" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK7" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL7" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM7" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN7" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO7" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP7" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ7" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT7" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV7" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AW7" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX7" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="AY7" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:51" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="S8" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="T8" s="13">
-        <v>41052</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="V8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="W8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="X8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z8" s="13">
-        <v>33381</v>
-      </c>
-      <c r="AA8" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB8" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG8" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH8" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI8" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ8" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK8" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL8" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="AM8" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN8" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO8" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP8" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ8" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR8" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AT8" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AU8" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV8" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AW8" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX8" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="AY8" s="9" t="s">
+      <c r="BB3" s="9" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N3" r:id="rId1" xr:uid="{F891FF0F-5644-48DA-804C-02A8681B37A7}"/>
-    <hyperlink ref="N4" r:id="rId2" xr:uid="{715B6D86-36E5-40DF-BD42-71200F4F6736}"/>
-    <hyperlink ref="N5" r:id="rId3" xr:uid="{5D052794-8876-4C6A-A6E2-E8FA359228E5}"/>
-    <hyperlink ref="N6" r:id="rId4" xr:uid="{FA5F4D37-FA0F-47A7-99AE-BEF14BA13095}"/>
-    <hyperlink ref="N7" r:id="rId5" xr:uid="{93124712-A4E6-4D44-9073-D4EB458DF516}"/>
-    <hyperlink ref="N8" r:id="rId6" xr:uid="{79880483-7DAC-4659-893D-BF48D915A0B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2631,21 +1928,21 @@
   <dimension ref="A1:AU6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.26953125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="15.26953125" style="14"/>
+    <col min="1" max="16384" width="15.26953125" style="14" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2976,10 +2273,10 @@
     </row>
     <row r="4" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="29"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -3157,39 +2454,46 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB8217E-4CD9-4CE8-B210-279243651323}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.90625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="38.453125" style="14" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.7265625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="B1" s="28"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="14">
         <v>2000006416</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="14">
         <v>2000006844</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="14">
         <v>2000007330</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified the script for key value pair
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XC2\marquisfinance\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradeep\Marquis\Master download\8-2-2023\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F77C9E-0AE9-42FF-B27D-D148BB7BEBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686A91AE-E1CD-406A-BF41-BEEEF993FD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="90" windowWidth="17520" windowHeight="9990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="804" yWindow="804" windowWidth="21600" windowHeight="11112" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="131">
   <si>
     <t>Dealer Group</t>
   </si>
@@ -404,6 +404,24 @@
   </si>
   <si>
     <t>MR</t>
+  </si>
+  <si>
+    <t>ReferenceNo1</t>
+  </si>
+  <si>
+    <t>ReferenceNo2</t>
+  </si>
+  <si>
+    <t>ReferenceNo3</t>
+  </si>
+  <si>
+    <t>2000006494</t>
+  </si>
+  <si>
+    <t>2000006844</t>
+  </si>
+  <si>
+    <t>2000007330</t>
   </si>
 </sst>
 </file>
@@ -894,19 +912,19 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="31"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -914,7 +932,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -922,13 +940,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -936,7 +954,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -963,18 +981,18 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="16.81640625" style="2" collapsed="1"/>
+    <col min="1" max="16384" width="16.77734375" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15"/>
       <c r="G1" s="17" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:53" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="25" t="s">
         <v>0</v>
@@ -1133,7 +1151,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
       <c r="B3" s="25" t="s">
         <v>1</v>
@@ -1290,83 +1308,83 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M4" s="3"/>
       <c r="T4" s="4"/>
       <c r="Y4" s="3"/>
       <c r="AI4" s="3"/>
       <c r="AT4" s="3"/>
     </row>
-    <row r="5" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="AI5" s="3"/>
       <c r="AT5" s="3"/>
     </row>
-    <row r="6" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="AI6" s="3"/>
       <c r="AT6" s="3"/>
     </row>
-    <row r="7" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M7" s="3"/>
       <c r="T7" s="5"/>
       <c r="Y7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AT7" s="3"/>
     </row>
-    <row r="8" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M8" s="3"/>
       <c r="T8" s="5"/>
       <c r="Y8" s="3"/>
       <c r="AI8" s="3"/>
       <c r="AT8" s="3"/>
     </row>
-    <row r="9" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M9" s="3"/>
       <c r="T9" s="5"/>
       <c r="Y9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AT9" s="3"/>
     </row>
-    <row r="10" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="AI10" s="3"/>
     </row>
-    <row r="11" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="AI11" s="3"/>
       <c r="AT11" s="3"/>
     </row>
-    <row r="12" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="AI12" s="3"/>
       <c r="AT12" s="3"/>
     </row>
-    <row r="13" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M13" s="3"/>
       <c r="T13" s="4"/>
       <c r="Y13" s="3"/>
       <c r="AI13" s="3"/>
       <c r="AT13" s="3"/>
     </row>
-    <row r="14" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="AI14" s="3"/>
       <c r="AT14" s="3"/>
     </row>
-    <row r="15" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="AI15" s="3"/>
       <c r="AT15" s="3"/>
     </row>
-    <row r="16" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="AI16" s="3"/>
@@ -1374,7 +1392,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="AI17" s="3"/>
@@ -1382,148 +1400,148 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M19" s="3"/>
       <c r="T19" s="4"/>
       <c r="Y19" s="3"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M20" s="3"/>
       <c r="T20" s="5"/>
       <c r="Y20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M21" s="3"/>
       <c r="T21" s="5"/>
       <c r="Y21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
-    <row r="22" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M22" s="3"/>
       <c r="Q22" s="5"/>
       <c r="T22" s="5"/>
       <c r="Y22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
-    <row r="23" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M23" s="3"/>
       <c r="Y23" s="3"/>
     </row>
-    <row r="24" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M25" s="3"/>
       <c r="T25" s="6"/>
       <c r="Y25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
-    <row r="26" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M26" s="3"/>
       <c r="T26" s="5"/>
       <c r="Y26" s="3"/>
       <c r="AI26" s="3"/>
     </row>
-    <row r="27" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M27" s="3"/>
       <c r="T27" s="5"/>
       <c r="Y27" s="3"/>
       <c r="AI27" s="3"/>
     </row>
-    <row r="28" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M28" s="3"/>
       <c r="T28" s="5"/>
       <c r="Y28" s="3"/>
       <c r="AI28" s="3"/>
     </row>
-    <row r="29" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M29" s="3"/>
       <c r="T29" s="5"/>
       <c r="Y29" s="3"/>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M30" s="3"/>
       <c r="T30" s="5"/>
     </row>
-    <row r="31" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M31" s="3"/>
       <c r="T31" s="5"/>
       <c r="Y31" s="3"/>
     </row>
-    <row r="32" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M32" s="3"/>
       <c r="T32" s="5"/>
       <c r="Y32" s="3"/>
     </row>
-    <row r="33" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M33" s="3"/>
       <c r="T33" s="5"/>
       <c r="Y33" s="3"/>
     </row>
-    <row r="34" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M34" s="3"/>
       <c r="T34" s="5"/>
       <c r="Y34" s="3"/>
     </row>
-    <row r="35" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M35" s="3"/>
       <c r="T35" s="5"/>
       <c r="Y35" s="3"/>
     </row>
-    <row r="36" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M36" s="3"/>
       <c r="T36" s="5"/>
       <c r="Y36" s="3"/>
     </row>
-    <row r="37" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M37" s="3"/>
       <c r="T37" s="5"/>
     </row>
-    <row r="38" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M39" s="3"/>
       <c r="T39" s="5"/>
     </row>
-    <row r="40" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M40" s="3"/>
       <c r="T40" s="5"/>
     </row>
-    <row r="41" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M41" s="3"/>
       <c r="T41" s="5"/>
     </row>
-    <row r="42" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="T42" s="5"/>
     </row>
-    <row r="43" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M43" s="3"/>
       <c r="T43" s="5"/>
     </row>
-    <row r="44" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M48" s="3"/>
     </row>
   </sheetData>
@@ -1537,59 +1555,61 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA63286-C133-4451-909B-35F8FE7B40BE}">
-  <dimension ref="A1:BB3"/>
+  <dimension ref="A1:BE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AZ3" sqref="AZ3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="BB8" sqref="BB8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="9.26953125" style="17" collapsed="1"/>
-    <col min="4" max="4" width="12.08984375" style="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.36328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.36328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="9.26953125" style="17" collapsed="1"/>
-    <col min="9" max="9" width="16.7265625" style="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.26953125" style="17" collapsed="1"/>
-    <col min="11" max="11" width="10.1796875" style="17" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.1796875" style="17" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.36328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.1796875" style="17" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="9.26953125" style="17" collapsed="1"/>
-    <col min="17" max="17" width="18.26953125" style="17" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="9.26953125" style="17" collapsed="1"/>
-    <col min="20" max="20" width="9.26953125" style="2" collapsed="1"/>
-    <col min="21" max="25" width="9.26953125" style="17" collapsed="1"/>
-    <col min="26" max="26" width="9.453125" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="32" width="9.26953125" style="17" collapsed="1"/>
-    <col min="33" max="33" width="10.6328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.26953125" style="17" collapsed="1"/>
-    <col min="35" max="35" width="10.7265625" style="17" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.26953125" style="17" collapsed="1"/>
-    <col min="37" max="37" width="11.1796875" style="17" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="9.21875" style="17" collapsed="1"/>
+    <col min="4" max="4" width="12.109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.33203125" style="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.33203125" style="17" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="9.21875" style="17" collapsed="1"/>
+    <col min="9" max="9" width="16.77734375" style="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.21875" style="17" collapsed="1"/>
+    <col min="11" max="11" width="10.21875" style="17" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.21875" style="17" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.33203125" style="17" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.21875" style="17" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="9.21875" style="17" collapsed="1"/>
+    <col min="17" max="17" width="18.21875" style="17" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="9.21875" style="17" collapsed="1"/>
+    <col min="20" max="20" width="9.21875" style="2" collapsed="1"/>
+    <col min="21" max="25" width="9.21875" style="17" collapsed="1"/>
+    <col min="26" max="26" width="9.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="32" width="9.21875" style="17" collapsed="1"/>
+    <col min="33" max="33" width="10.6640625" style="17" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="9.21875" style="17" collapsed="1"/>
+    <col min="35" max="35" width="10.77734375" style="17" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.21875" style="17" collapsed="1"/>
+    <col min="37" max="37" width="11.21875" style="17" customWidth="1" collapsed="1"/>
     <col min="38" max="38" width="13" style="17" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="17.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="40" max="42" width="12.08984375" style="17" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="16.453125" style="17" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="9.26953125" style="17" collapsed="1"/>
+    <col min="39" max="39" width="17.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="40" max="42" width="12.109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="16.44140625" style="17" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="9.21875" style="17" collapsed="1"/>
     <col min="45" max="45" width="16" style="17" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="14.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="9.26953125" style="17" collapsed="1"/>
-    <col min="49" max="49" width="15.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="13.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="20.6328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="53" max="16384" width="9.26953125" style="17" collapsed="1"/>
+    <col min="46" max="46" width="14.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="9.21875" style="17" collapsed="1"/>
+    <col min="49" max="49" width="15.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="13.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="20.6640625" style="17" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="53" max="54" width="9.21875" style="17" collapsed="1"/>
+    <col min="55" max="57" width="11" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="16384" width="9.21875" style="17" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:57" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F1" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:57" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
@@ -1752,8 +1772,17 @@
       <c r="BB2" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:54" ht="58" x14ac:dyDescent="0.35">
+      <c r="BC2" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="BD2" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="BE2" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:57" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
@@ -1913,6 +1942,15 @@
       </c>
       <c r="BB3" s="9" t="s">
         <v>104</v>
+      </c>
+      <c r="BC3" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="BD3" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE3" s="19" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1931,12 +1969,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.26953125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15.21875" defaultRowHeight="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="15.26953125" style="14" collapsed="1"/>
+    <col min="1" max="16384" width="15.21875" style="14" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>101</v>
       </c>
@@ -1987,7 +2025,7 @@
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
     </row>
-    <row r="2" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
@@ -2130,7 +2168,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>97</v>
       </c>
@@ -2271,7 +2309,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="33" t="s">
         <v>83</v>
@@ -2322,7 +2360,7 @@
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
     </row>
-    <row r="5" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2381,7 +2419,7 @@
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
     </row>
-    <row r="6" spans="1:47" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" ht="44.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -2460,39 +2498,39 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.453125" style="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.7265625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.54296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="38.44140625" style="14" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>71</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>2000006416</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>2000006844</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>2000007330</v>
       </c>

</xml_diff>

<commit_message>
Added scripts for multiple Run
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradeep\Marquis\Master download\8-2-2023\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backup\fEB 14\marquisfinance\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686A91AE-E1CD-406A-BF41-BEEEF993FD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7A252CB-CA60-4FEC-A2B9-5314E689D7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="804" yWindow="804" windowWidth="21600" windowHeight="11112" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="0" windowWidth="17520" windowHeight="9990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="7" r:id="rId1"/>
     <sheet name="TestDataOLD" sheetId="1" r:id="rId2"/>
     <sheet name="TestData" sheetId="9" r:id="rId3"/>
-    <sheet name="old" sheetId="8" r:id="rId4"/>
+    <sheet name="CusotmerDetails" sheetId="8" r:id="rId4"/>
     <sheet name="RefNumber" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="135">
   <si>
     <t>Dealer Group</t>
   </si>
@@ -364,6 +364,9 @@
     <t>userID</t>
   </si>
   <si>
+    <t>Transaction Number</t>
+  </si>
+  <si>
     <t>InterestRateType</t>
   </si>
   <si>
@@ -385,43 +388,52 @@
     <t>150000</t>
   </si>
   <si>
-    <t>27 Feb 2023</t>
-  </si>
-  <si>
     <t>FIXED</t>
   </si>
   <si>
     <t>195,000.00</t>
   </si>
   <si>
-    <t>6301045178080</t>
-  </si>
-  <si>
-    <t>VENESH</t>
-  </si>
-  <si>
-    <t>SEWSUNKER</t>
-  </si>
-  <si>
     <t>MR</t>
   </si>
   <si>
-    <t>ReferenceNo1</t>
-  </si>
-  <si>
-    <t>ReferenceNo2</t>
-  </si>
-  <si>
-    <t>ReferenceNo3</t>
-  </si>
-  <si>
-    <t>2000006494</t>
-  </si>
-  <si>
-    <t>2000006844</t>
-  </si>
-  <si>
-    <t>2000007330</t>
+    <t>27 Mar 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Name </t>
+  </si>
+  <si>
+    <t>6607045088081</t>
+  </si>
+  <si>
+    <t>ETTIENE</t>
+  </si>
+  <si>
+    <t>SMITH</t>
+  </si>
+  <si>
+    <t>6607135266084</t>
+  </si>
+  <si>
+    <t>TERENCE</t>
+  </si>
+  <si>
+    <t>PIENAAR</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>2000007544</t>
+  </si>
+  <si>
+    <t>2000007551</t>
+  </si>
+  <si>
+    <t>63292</t>
+  </si>
+  <si>
+    <t>2000007552</t>
   </si>
 </sst>
 </file>
@@ -511,13 +523,9 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -610,10 +618,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -624,6 +629,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -912,19 +920,19 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="31"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="30"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -932,7 +940,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -940,13 +948,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -954,7 +962,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -978,21 +986,21 @@
   <dimension ref="A1:BA48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="AU5" sqref="AU5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="16.77734375" style="2" collapsed="1"/>
+    <col min="1" max="16384" width="16.81640625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15"/>
       <c r="G1" s="17" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="25" t="s">
         <v>0</v>
@@ -1151,7 +1159,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
       <c r="B3" s="25" t="s">
         <v>1</v>
@@ -1308,83 +1316,83 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M4" s="3"/>
       <c r="T4" s="4"/>
       <c r="Y4" s="3"/>
       <c r="AI4" s="3"/>
       <c r="AT4" s="3"/>
     </row>
-    <row r="5" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="AI5" s="3"/>
       <c r="AT5" s="3"/>
     </row>
-    <row r="6" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="AI6" s="3"/>
       <c r="AT6" s="3"/>
     </row>
-    <row r="7" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M7" s="3"/>
       <c r="T7" s="5"/>
       <c r="Y7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AT7" s="3"/>
     </row>
-    <row r="8" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M8" s="3"/>
       <c r="T8" s="5"/>
       <c r="Y8" s="3"/>
       <c r="AI8" s="3"/>
       <c r="AT8" s="3"/>
     </row>
-    <row r="9" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M9" s="3"/>
       <c r="T9" s="5"/>
       <c r="Y9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AT9" s="3"/>
     </row>
-    <row r="10" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="AI10" s="3"/>
     </row>
-    <row r="11" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="AI11" s="3"/>
       <c r="AT11" s="3"/>
     </row>
-    <row r="12" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="AI12" s="3"/>
       <c r="AT12" s="3"/>
     </row>
-    <row r="13" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M13" s="3"/>
       <c r="T13" s="4"/>
       <c r="Y13" s="3"/>
       <c r="AI13" s="3"/>
       <c r="AT13" s="3"/>
     </row>
-    <row r="14" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="AI14" s="3"/>
       <c r="AT14" s="3"/>
     </row>
-    <row r="15" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="AI15" s="3"/>
       <c r="AT15" s="3"/>
     </row>
-    <row r="16" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="AI16" s="3"/>
@@ -1392,7 +1400,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="AI17" s="3"/>
@@ -1400,148 +1408,148 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M19" s="3"/>
       <c r="T19" s="4"/>
       <c r="Y19" s="3"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M20" s="3"/>
       <c r="T20" s="5"/>
       <c r="Y20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M21" s="3"/>
       <c r="T21" s="5"/>
       <c r="Y21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
-    <row r="22" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M22" s="3"/>
       <c r="Q22" s="5"/>
       <c r="T22" s="5"/>
       <c r="Y22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
-    <row r="23" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M23" s="3"/>
       <c r="Y23" s="3"/>
     </row>
-    <row r="24" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M25" s="3"/>
       <c r="T25" s="6"/>
       <c r="Y25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
-    <row r="26" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M26" s="3"/>
       <c r="T26" s="5"/>
       <c r="Y26" s="3"/>
       <c r="AI26" s="3"/>
     </row>
-    <row r="27" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M27" s="3"/>
       <c r="T27" s="5"/>
       <c r="Y27" s="3"/>
       <c r="AI27" s="3"/>
     </row>
-    <row r="28" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M28" s="3"/>
       <c r="T28" s="5"/>
       <c r="Y28" s="3"/>
       <c r="AI28" s="3"/>
     </row>
-    <row r="29" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M29" s="3"/>
       <c r="T29" s="5"/>
       <c r="Y29" s="3"/>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M30" s="3"/>
       <c r="T30" s="5"/>
     </row>
-    <row r="31" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M31" s="3"/>
       <c r="T31" s="5"/>
       <c r="Y31" s="3"/>
     </row>
-    <row r="32" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M32" s="3"/>
       <c r="T32" s="5"/>
       <c r="Y32" s="3"/>
     </row>
-    <row r="33" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M33" s="3"/>
       <c r="T33" s="5"/>
       <c r="Y33" s="3"/>
     </row>
-    <row r="34" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M34" s="3"/>
       <c r="T34" s="5"/>
       <c r="Y34" s="3"/>
     </row>
-    <row r="35" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M35" s="3"/>
       <c r="T35" s="5"/>
       <c r="Y35" s="3"/>
     </row>
-    <row r="36" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M36" s="3"/>
       <c r="T36" s="5"/>
       <c r="Y36" s="3"/>
     </row>
-    <row r="37" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M37" s="3"/>
       <c r="T37" s="5"/>
     </row>
-    <row r="38" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M39" s="3"/>
       <c r="T39" s="5"/>
     </row>
-    <row r="40" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M40" s="3"/>
       <c r="T40" s="5"/>
     </row>
-    <row r="41" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M41" s="3"/>
       <c r="T41" s="5"/>
     </row>
-    <row r="42" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="T42" s="5"/>
     </row>
-    <row r="43" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M43" s="3"/>
       <c r="T43" s="5"/>
     </row>
-    <row r="44" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M48" s="3"/>
     </row>
   </sheetData>
@@ -1555,61 +1563,59 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA63286-C133-4451-909B-35F8FE7B40BE}">
-  <dimension ref="A1:BE3"/>
+  <dimension ref="A1:BB4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="BB8" sqref="BB8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="9.21875" style="17" collapsed="1"/>
-    <col min="4" max="4" width="12.109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.33203125" style="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.33203125" style="17" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="9.21875" style="17" collapsed="1"/>
-    <col min="9" max="9" width="16.77734375" style="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.21875" style="17" collapsed="1"/>
-    <col min="11" max="11" width="10.21875" style="17" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.21875" style="17" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.33203125" style="17" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.21875" style="17" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="9.21875" style="17" collapsed="1"/>
-    <col min="17" max="17" width="18.21875" style="17" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="9.21875" style="17" collapsed="1"/>
-    <col min="20" max="20" width="9.21875" style="2" collapsed="1"/>
-    <col min="21" max="25" width="9.21875" style="17" collapsed="1"/>
-    <col min="26" max="26" width="9.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="32" width="9.21875" style="17" collapsed="1"/>
-    <col min="33" max="33" width="10.6640625" style="17" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.21875" style="17" collapsed="1"/>
-    <col min="35" max="35" width="10.77734375" style="17" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.21875" style="17" collapsed="1"/>
-    <col min="37" max="37" width="11.21875" style="17" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="9.26953125" style="17" collapsed="1"/>
+    <col min="4" max="4" width="12.08984375" style="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.36328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.36328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="9.26953125" style="17" collapsed="1"/>
+    <col min="9" max="9" width="16.7265625" style="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.26953125" style="17" collapsed="1"/>
+    <col min="11" max="11" width="10.1796875" style="17" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.1796875" style="17" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.36328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.1796875" style="17" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="9.26953125" style="17" collapsed="1"/>
+    <col min="17" max="17" width="18.26953125" style="17" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="9.26953125" style="17" collapsed="1"/>
+    <col min="20" max="20" width="9.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="25" width="9.26953125" style="17" collapsed="1"/>
+    <col min="26" max="26" width="9.453125" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="32" width="9.26953125" style="17" collapsed="1"/>
+    <col min="33" max="33" width="10.6328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="9.26953125" style="17" collapsed="1"/>
+    <col min="35" max="35" width="10.7265625" style="17" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.26953125" style="17" collapsed="1"/>
+    <col min="37" max="37" width="11.1796875" style="17" customWidth="1" collapsed="1"/>
     <col min="38" max="38" width="13" style="17" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="17.5546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="40" max="42" width="12.109375" style="17" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="16.44140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="9.21875" style="17" collapsed="1"/>
+    <col min="39" max="39" width="17.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="40" max="42" width="12.08984375" style="17" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="16.453125" style="17" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="9.26953125" style="17" collapsed="1"/>
     <col min="45" max="45" width="16" style="17" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="14.5546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="9.21875" style="17" collapsed="1"/>
-    <col min="49" max="49" width="15.5546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="13.5546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="20.6640625" style="17" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12.5546875" style="17" customWidth="1" collapsed="1"/>
-    <col min="53" max="54" width="9.21875" style="17" collapsed="1"/>
-    <col min="55" max="57" width="11" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="16384" width="9.21875" style="17" collapsed="1"/>
+    <col min="46" max="46" width="14.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="9.26953125" style="17" collapsed="1"/>
+    <col min="49" max="49" width="15.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="13.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="20.6328125" style="17" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.54296875" style="17" customWidth="1" collapsed="1"/>
+    <col min="53" max="16384" width="9.26953125" style="17" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="F1" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:57" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
@@ -1731,10 +1737,10 @@
         <v>53</v>
       </c>
       <c r="AO2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP2" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="AP2" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="AQ2" s="10" t="s">
         <v>57</v>
@@ -1761,7 +1767,7 @@
         <v>102</v>
       </c>
       <c r="AY2" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AZ2" s="10" t="s">
         <v>78</v>
@@ -1772,17 +1778,8 @@
       <c r="BB2" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="BC2" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="BD2" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="BE2" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:57" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:54" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
@@ -1793,22 +1790,22 @@
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>46</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>40</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="10" t="s">
@@ -1863,10 +1860,10 @@
         <v>54</v>
       </c>
       <c r="AB3" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AC3" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AD3" s="10" t="s">
         <v>37</v>
@@ -1896,13 +1893,13 @@
         <v>94</v>
       </c>
       <c r="AM3" s="9" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="AN3" s="9" t="s">
         <v>76</v>
       </c>
       <c r="AO3" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AP3" s="9" t="s">
         <v>119</v>
@@ -1932,7 +1929,7 @@
         <v>99</v>
       </c>
       <c r="AY3" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AZ3" s="9" t="s">
         <v>79</v>
@@ -1943,19 +1940,173 @@
       <c r="BB3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="BC3" s="19" t="s">
+    </row>
+    <row r="4" spans="1:54" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="BD3" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="BE3" s="19" t="s">
-        <v>130</v>
+      <c r="G4" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="T4" s="13">
+        <v>41052</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z4" s="13">
+        <v>36303</v>
+      </c>
+      <c r="AA4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG4" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL4" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM4" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO4" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP4" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AQ4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS4" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW4" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AX4" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AY4" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="AZ4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB4" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="N3" r:id="rId1" xr:uid="{F891FF0F-5644-48DA-804C-02A8681B37A7}"/>
+    <hyperlink ref="N4" r:id="rId2" xr:uid="{EF14D0D0-F702-44A7-988C-3B068070596A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1966,21 +2117,21 @@
   <dimension ref="A1:AU6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.21875" defaultRowHeight="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15.26953125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="15.21875" style="14" collapsed="1"/>
+    <col min="1" max="16384" width="15.26953125" style="14" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2025,7 +2176,7 @@
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
     </row>
-    <row r="2" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
@@ -2168,7 +2319,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>97</v>
       </c>
@@ -2309,12 +2460,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2360,7 +2511,7 @@
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
     </row>
-    <row r="5" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2419,7 +2570,7 @@
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
     </row>
-    <row r="6" spans="1:47" ht="44.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:47" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -2492,50 +2643,394 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EB8217E-4CD9-4CE8-B210-279243651323}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" style="14" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.77734375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="38.453125" style="14" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7265625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.7265625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="14">
-        <v>2000006416</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
-        <v>2000006844</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
-        <v>2000007330</v>
-      </c>
+      <c r="B2" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="29">
+        <v>63292</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="28"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="28"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="28"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="28"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="28"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="28"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="28"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="28"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="28"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="28"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="28"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reduced the wait of verify buttons
</commit_message>
<xml_diff>
--- a/XLSX/MarquisDataForm.xlsx
+++ b/XLSX/MarquisDataForm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XC3\marquisfinance\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pradeep\Marquis\Master download\23-02-2023\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BE0DFA-855C-47AF-8A55-9C4EC254E43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996AEE44-FF5F-46D7-8E57-47E05A6C2C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="90" windowWidth="17520" windowHeight="9990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="21600" windowHeight="11112" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="RefNumber" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -445,7 +446,7 @@
     <t>59229</t>
   </si>
   <si>
-    <t>2000006991</t>
+    <t>2000007637</t>
   </si>
 </sst>
 </file>
@@ -636,6 +637,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -648,7 +650,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -936,19 +937,19 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="31"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="32"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -956,7 +957,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -964,13 +965,13 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -978,7 +979,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -1005,18 +1006,18 @@
       <selection activeCell="AU5" sqref="AU5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="16.81640625" style="2" collapsed="1"/>
+    <col min="1" max="16384" width="16.77734375" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15"/>
       <c r="G1" s="17" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:53" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="25" t="s">
         <v>0</v>
@@ -1175,7 +1176,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:53" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15"/>
       <c r="B3" s="25" t="s">
         <v>1</v>
@@ -1332,83 +1333,83 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M4" s="3"/>
       <c r="T4" s="4"/>
       <c r="Y4" s="3"/>
       <c r="AI4" s="3"/>
       <c r="AT4" s="3"/>
     </row>
-    <row r="5" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="AI5" s="3"/>
       <c r="AT5" s="3"/>
     </row>
-    <row r="6" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="AI6" s="3"/>
       <c r="AT6" s="3"/>
     </row>
-    <row r="7" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M7" s="3"/>
       <c r="T7" s="5"/>
       <c r="Y7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AT7" s="3"/>
     </row>
-    <row r="8" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M8" s="3"/>
       <c r="T8" s="5"/>
       <c r="Y8" s="3"/>
       <c r="AI8" s="3"/>
       <c r="AT8" s="3"/>
     </row>
-    <row r="9" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M9" s="3"/>
       <c r="T9" s="5"/>
       <c r="Y9" s="3"/>
       <c r="AI9" s="3"/>
       <c r="AT9" s="3"/>
     </row>
-    <row r="10" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="AI10" s="3"/>
     </row>
-    <row r="11" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="AI11" s="3"/>
       <c r="AT11" s="3"/>
     </row>
-    <row r="12" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="AI12" s="3"/>
       <c r="AT12" s="3"/>
     </row>
-    <row r="13" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M13" s="3"/>
       <c r="T13" s="4"/>
       <c r="Y13" s="3"/>
       <c r="AI13" s="3"/>
       <c r="AT13" s="3"/>
     </row>
-    <row r="14" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M14" s="3"/>
       <c r="Y14" s="3"/>
       <c r="AI14" s="3"/>
       <c r="AT14" s="3"/>
     </row>
-    <row r="15" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="AI15" s="3"/>
       <c r="AT15" s="3"/>
     </row>
-    <row r="16" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:53" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="AI16" s="3"/>
@@ -1416,7 +1417,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="AI17" s="3"/>
@@ -1424,148 +1425,148 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="AI18" s="3"/>
     </row>
-    <row r="19" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M19" s="3"/>
       <c r="T19" s="4"/>
       <c r="Y19" s="3"/>
       <c r="AI19" s="3"/>
     </row>
-    <row r="20" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M20" s="3"/>
       <c r="T20" s="5"/>
       <c r="Y20" s="3"/>
       <c r="AI20" s="3"/>
     </row>
-    <row r="21" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M21" s="3"/>
       <c r="T21" s="5"/>
       <c r="Y21" s="3"/>
       <c r="AI21" s="3"/>
     </row>
-    <row r="22" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M22" s="3"/>
       <c r="Q22" s="5"/>
       <c r="T22" s="5"/>
       <c r="Y22" s="3"/>
       <c r="AI22" s="3"/>
     </row>
-    <row r="23" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M23" s="3"/>
       <c r="Y23" s="3"/>
     </row>
-    <row r="24" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="AI24" s="3"/>
     </row>
-    <row r="25" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M25" s="3"/>
       <c r="T25" s="6"/>
       <c r="Y25" s="3"/>
       <c r="AI25" s="3"/>
     </row>
-    <row r="26" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M26" s="3"/>
       <c r="T26" s="5"/>
       <c r="Y26" s="3"/>
       <c r="AI26" s="3"/>
     </row>
-    <row r="27" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M27" s="3"/>
       <c r="T27" s="5"/>
       <c r="Y27" s="3"/>
       <c r="AI27" s="3"/>
     </row>
-    <row r="28" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M28" s="3"/>
       <c r="T28" s="5"/>
       <c r="Y28" s="3"/>
       <c r="AI28" s="3"/>
     </row>
-    <row r="29" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M29" s="3"/>
       <c r="T29" s="5"/>
       <c r="Y29" s="3"/>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M30" s="3"/>
       <c r="T30" s="5"/>
     </row>
-    <row r="31" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M31" s="3"/>
       <c r="T31" s="5"/>
       <c r="Y31" s="3"/>
     </row>
-    <row r="32" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="13:46" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M32" s="3"/>
       <c r="T32" s="5"/>
       <c r="Y32" s="3"/>
     </row>
-    <row r="33" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M33" s="3"/>
       <c r="T33" s="5"/>
       <c r="Y33" s="3"/>
     </row>
-    <row r="34" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M34" s="3"/>
       <c r="T34" s="5"/>
       <c r="Y34" s="3"/>
     </row>
-    <row r="35" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M35" s="3"/>
       <c r="T35" s="5"/>
       <c r="Y35" s="3"/>
     </row>
-    <row r="36" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M36" s="3"/>
       <c r="T36" s="5"/>
       <c r="Y36" s="3"/>
     </row>
-    <row r="37" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M37" s="3"/>
       <c r="T37" s="5"/>
     </row>
-    <row r="38" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M39" s="3"/>
       <c r="T39" s="5"/>
     </row>
-    <row r="40" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M40" s="3"/>
       <c r="T40" s="5"/>
     </row>
-    <row r="41" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M41" s="3"/>
       <c r="T41" s="5"/>
     </row>
-    <row r="42" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="T42" s="5"/>
     </row>
-    <row r="43" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M43" s="3"/>
       <c r="T43" s="5"/>
     </row>
-    <row r="44" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="13:25" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="M48" s="3"/>
     </row>
   </sheetData>
@@ -1585,53 +1586,53 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="9.26953125" style="17" collapsed="1"/>
-    <col min="4" max="4" width="12.08984375" style="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.36328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.36328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="9.26953125" style="17" collapsed="1"/>
-    <col min="9" max="9" width="16.7265625" style="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.26953125" style="17" collapsed="1"/>
-    <col min="11" max="11" width="10.1796875" style="17" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.1796875" style="17" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.36328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.1796875" style="17" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="9.26953125" style="17" collapsed="1"/>
-    <col min="17" max="17" width="18.26953125" style="17" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="9.26953125" style="17" collapsed="1"/>
-    <col min="20" max="20" width="9.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="25" width="9.26953125" style="17" collapsed="1"/>
-    <col min="26" max="26" width="9.453125" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="32" width="9.26953125" style="17" collapsed="1"/>
-    <col min="33" max="33" width="10.6328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.26953125" style="17" collapsed="1"/>
-    <col min="35" max="35" width="10.7265625" style="17" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="9.26953125" style="17" collapsed="1"/>
-    <col min="37" max="37" width="11.1796875" style="17" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="9.21875" style="17" collapsed="1"/>
+    <col min="4" max="4" width="12.109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.33203125" style="17" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.33203125" style="17" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="9.21875" style="17" collapsed="1"/>
+    <col min="9" max="9" width="16.77734375" style="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.21875" style="17" collapsed="1"/>
+    <col min="11" max="11" width="10.21875" style="17" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.21875" style="17" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.33203125" style="17" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.21875" style="17" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="9.21875" style="17" collapsed="1"/>
+    <col min="17" max="17" width="18.21875" style="17" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="9.21875" style="17" collapsed="1"/>
+    <col min="20" max="20" width="9.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="25" width="9.21875" style="17" collapsed="1"/>
+    <col min="26" max="26" width="9.44140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="32" width="9.21875" style="17" collapsed="1"/>
+    <col min="33" max="33" width="10.6640625" style="17" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="9.21875" style="17" collapsed="1"/>
+    <col min="35" max="35" width="10.77734375" style="17" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="9.21875" style="17" collapsed="1"/>
+    <col min="37" max="37" width="11.21875" style="17" customWidth="1" collapsed="1"/>
     <col min="38" max="38" width="13" style="17" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="17.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="40" max="42" width="12.08984375" style="17" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="16.453125" style="17" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="9.26953125" style="17" collapsed="1"/>
+    <col min="39" max="39" width="17.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="40" max="42" width="12.109375" style="17" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="16.44140625" style="17" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="9.21875" style="17" collapsed="1"/>
     <col min="45" max="45" width="16" style="17" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="14.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="9.26953125" style="17" collapsed="1"/>
-    <col min="49" max="49" width="15.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="13.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="20.6328125" style="17" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12.54296875" style="17" customWidth="1" collapsed="1"/>
-    <col min="53" max="16384" width="9.26953125" style="17" collapsed="1"/>
+    <col min="46" max="46" width="14.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="9.21875" style="17" collapsed="1"/>
+    <col min="49" max="49" width="15.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="13.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="20.6640625" style="17" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="12.5546875" style="17" customWidth="1" collapsed="1"/>
+    <col min="53" max="16384" width="9.21875" style="17" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:54" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F1" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:54" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:54" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:54" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:54" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
         <v>1</v>
       </c>
@@ -2136,18 +2137,18 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.26953125" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15.21875" defaultRowHeight="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="15.26953125" style="14" collapsed="1"/>
+    <col min="1" max="16384" width="15.21875" style="14" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2192,7 +2193,7 @@
       <c r="AT1" s="2"/>
       <c r="AU1" s="2"/>
     </row>
-    <row r="2" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
@@ -2335,7 +2336,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>97</v>
       </c>
@@ -2476,12 +2477,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2527,7 +2528,7 @@
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
     </row>
-    <row r="5" spans="1:47" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:47" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -2586,7 +2587,7 @@
       <c r="AT5" s="2"/>
       <c r="AU5" s="2"/>
     </row>
-    <row r="6" spans="1:47" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:47" ht="44.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -2662,36 +2663,36 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.453125" style="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="38.44140625" style="14" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="23" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7265625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7265625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="35" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>71</v>
       </c>
@@ -2708,18 +2709,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="31" t="s">
         <v>137</v>
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>133</v>
       </c>
@@ -2736,7 +2737,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>135</v>
       </c>
@@ -2753,301 +2754,301 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="28"/>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="28"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="28"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="28"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="28"/>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="28"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29"/>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="28"/>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29"/>
       <c r="E12" s="29"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="28"/>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="29"/>
       <c r="E13" s="29"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="28"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29"/>
       <c r="E14" s="29"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="28"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="28"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="28"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
       <c r="D17" s="29"/>
       <c r="E17" s="29"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="28"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="28"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="28"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="29"/>
       <c r="E20" s="29"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="28"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="28"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="28"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="28"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="28"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="28"/>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="28"/>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="28"/>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="28"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
       <c r="E29" s="29"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="28"/>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
       <c r="D30" s="29"/>
       <c r="E30" s="29"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="28"/>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
       <c r="D31" s="29"/>
       <c r="E31" s="29"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="28"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
       <c r="E32" s="29"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="28"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="28"/>
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
       <c r="D34" s="29"/>
       <c r="E34" s="29"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="28"/>
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>
       <c r="D35" s="29"/>
       <c r="E35" s="29"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="28"/>
       <c r="B36" s="29"/>
       <c r="C36" s="29"/>
       <c r="D36" s="29"/>
       <c r="E36" s="29"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="28"/>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
       <c r="E37" s="29"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="28"/>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
       <c r="E38" s="29"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="28"/>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
       <c r="E39" s="29"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="28"/>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
       <c r="D40" s="29"/>
       <c r="E40" s="29"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="28"/>
       <c r="B41" s="29"/>
       <c r="C41" s="29"/>
       <c r="D41" s="29"/>
       <c r="E41" s="29"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="28"/>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
       <c r="D42" s="29"/>
       <c r="E42" s="29"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="28"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
       <c r="D43" s="29"/>
       <c r="E43" s="29"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="28"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="28"/>
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="28"/>
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>
       <c r="D46" s="29"/>
       <c r="E46" s="29"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="28"/>
       <c r="B47" s="29"/>
       <c r="C47" s="29"/>
       <c r="D47" s="29"/>
       <c r="E47" s="29"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="28"/>
       <c r="B48" s="29"/>
       <c r="C48" s="29"/>

</xml_diff>